<commit_message>
test case excel aktualisiert
</commit_message>
<xml_diff>
--- a/Testexercise2.xlsx
+++ b/Testexercise2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agil\TESTing Methoden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compi_000\PycharmProjects\Juicetest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CA8716-1358-4ECA-9F11-D25012028A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43B4D87-F151-4D88-82EE-FE6540D0240C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
+    <workbookView xWindow="22320" yWindow="2170" windowWidth="14400" windowHeight="7360" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
   </bookViews>
   <sheets>
     <sheet name="Juice_test" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>XXX buys 3 cartons</t>
+  </si>
+  <si>
+    <t>member must be boolean</t>
+  </si>
+  <si>
+    <t>"XXX"</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76080AAE-91CC-4536-8750-B6AE5B58BDF7}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,7 +576,7 @@
     <col min="1" max="1" width="6.1796875" style="9" customWidth="1"/>
     <col min="2" max="2" width="28.81640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="28.81640625" style="11" customWidth="1"/>
-    <col min="4" max="5" width="15.26953125" style="10" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="15.26953125" style="10" customWidth="1"/>
     <col min="6" max="6" width="10.90625" style="10"/>
     <col min="7" max="7" width="14.81640625" style="10" customWidth="1"/>
     <col min="8" max="16384" width="10.90625" style="10"/>
@@ -895,6 +904,12 @@
       <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="F13" s="7" t="s">
         <v>36</v>
       </c>
@@ -902,6 +917,32 @@
         <v>15</v>
       </c>
       <c r="H13" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>